<commit_message>
Code now passes all test :)
</commit_message>
<xml_diff>
--- a/ClueInitFiles/data/ClueLayout306.xlsx
+++ b/ClueInitFiles/data/ClueLayout306.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane Ritter\eclipse-workspace\ClueGame\ClueInitFiles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CF051C-790A-470F-8773-23B04C6E8EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E950C0D6-64AC-4C47-BEFD-EFCE3CE66ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2920" yWindow="4200" windowWidth="27150" windowHeight="14440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18010" yWindow="0" windowWidth="18280" windowHeight="19730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClueLayout" sheetId="1" r:id="rId1"/>
@@ -3130,7 +3130,7 @@
   <dimension ref="A1:X25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AQ10" sqref="AQ10"/>
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>